<commit_message>
MODIFICACION DE LA TABLAS  0072 0073 CAMBIO ACTIVO E INACTIVO EN ENUM PONER CAMPOS VACIOS Y AGRAGAR COMENTARIOS  Y DICCIONARIO DE INTEGRACIONES
</commit_message>
<xml_diff>
--- a/DICCIONARIOS/DICCIONARIO DE INTEGRACIONES.xlsx
+++ b/DICCIONARIOS/DICCIONARIO DE INTEGRACIONES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repremundo_Scripts\DICCIONARIOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53B9F62-6E81-4825-9D7E-CD4835E7F1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FFC33D-7DDA-443E-B652-8204D60A60EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5BCBB9E7-588B-48F5-92C5-53EE3EDF223B}"/>
   </bookViews>
@@ -491,7 +491,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -499,8 +499,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -836,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCCCBB4-D4DC-4E49-8F92-97CC01F2F54F}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,472 +848,592 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C27" t="s">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C28" t="s">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C29" t="s">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C30" t="s">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C33" t="s">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C34" t="s">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C35" t="s">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C36" t="s">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C37" t="s">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C38" t="s">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C39" t="s">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C40" t="s">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C41" t="s">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C42" t="s">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C43" t="s">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C44" t="s">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C45" t="s">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C46" t="s">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C47" t="s">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C48" t="s">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C49" t="s">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C50" t="s">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C51" t="s">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C52" t="s">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C53" t="s">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C54" t="s">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C55" t="s">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C56" t="s">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C57" t="s">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C58" t="s">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A27:A53">

</xml_diff>